<commit_message>
Also ran an exponential distribution
</commit_message>
<xml_diff>
--- a/DES/distributionResults.xlsx
+++ b/DES/distributionResults.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>servers</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>ss</t>
+  </si>
+  <si>
+    <t>Exponential distribution</t>
   </si>
 </sst>
 </file>
@@ -101,10 +104,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -438,91 +442,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17">
+    <row r="3" spans="1:5" ht="17">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
+        <v>52.947902323969799</v>
+      </c>
+      <c r="D3" s="2">
         <v>225569.26222046599</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>149740.05733049399</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17">
+    <row r="4" spans="1:5" ht="17">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
+        <v>44.162893299676398</v>
+      </c>
+      <c r="D4" s="2">
         <v>129956.723060284</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>86382.683362601005</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17">
+    <row r="5" spans="1:5" ht="17">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
+        <v>2.1911512597691098</v>
+      </c>
+      <c r="D5" s="2">
         <v>538.79623599768797</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>358.26010415643702</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17">
+    <row r="6" spans="1:5" ht="17">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
+        <v>0.93813258652195597</v>
+      </c>
+      <c r="D6" s="2">
         <v>44.252924375031</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>26.193638724849801</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17">
+    <row r="7" spans="1:5" ht="17">
       <c r="A7">
         <v>2</v>
       </c>
@@ -530,13 +551,16 @@
         <v>4</v>
       </c>
       <c r="C7" s="1">
+        <v>4.2279784780093102E-2</v>
+      </c>
+      <c r="D7" s="1">
         <v>104912.220439422</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>67722.966708097403</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17">
+    <row r="8" spans="1:5" ht="17">
       <c r="A8">
         <v>2</v>
       </c>
@@ -544,13 +568,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="1">
+        <v>1.0359324443449801E-2</v>
+      </c>
+      <c r="D8" s="1">
         <v>60642.989350169199</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>39004.312617370102</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17">
+    <row r="9" spans="1:5" ht="17">
       <c r="A9">
         <v>2</v>
       </c>
@@ -558,13 +585,16 @@
         <v>6</v>
       </c>
       <c r="C9" s="1">
+        <v>9.0423864873150198E-2</v>
+      </c>
+      <c r="D9" s="1">
         <v>251.709669571646</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>162.44144147346401</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17">
+    <row r="10" spans="1:5" ht="17">
       <c r="A10">
         <v>2</v>
       </c>
@@ -572,13 +602,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="1">
+        <v>2.0946151852236999E-2</v>
+      </c>
+      <c r="D10" s="1">
         <v>22.553671252861701</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>12.9469997073386</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17">
+    <row r="11" spans="1:5" ht="17">
       <c r="A11">
         <v>4</v>
       </c>
@@ -586,13 +619,16 @@
         <v>4</v>
       </c>
       <c r="C11" s="1">
+        <v>8.3081053291551095E-4</v>
+      </c>
+      <c r="D11" s="1">
         <v>44777.368940481203</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>26271.194566919199</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17">
+    <row r="12" spans="1:5" ht="17">
       <c r="A12">
         <v>4</v>
       </c>
@@ -600,13 +636,16 @@
         <v>5</v>
       </c>
       <c r="C12" s="1">
+        <v>4.8583102563977399E-4</v>
+      </c>
+      <c r="D12" s="1">
         <v>25826.104313972599</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>15150.657471050999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17">
+    <row r="13" spans="1:5" ht="17">
       <c r="A13">
         <v>4</v>
       </c>
@@ -614,13 +653,16 @@
         <v>6</v>
       </c>
       <c r="C13" s="1">
+        <v>7.5328932305506599E-3</v>
+      </c>
+      <c r="D13" s="1">
         <v>107.704667387314</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>62.8980383635419</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17">
+    <row r="14" spans="1:5" ht="17">
       <c r="A14">
         <v>4</v>
       </c>
@@ -628,65 +670,80 @@
         <v>7</v>
       </c>
       <c r="C14" s="1">
+        <v>3.3629020115662298E-3</v>
+      </c>
+      <c r="D14" s="1">
         <v>10.3373377318872</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>5.4421145594641098</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17">
+    <row r="15" spans="1:5" ht="17">
       <c r="A15">
         <v>8</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="3">
+        <v>2.0469768189286601E-7</v>
+      </c>
+      <c r="D15" s="1">
         <v>14972.739586018501</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>5538.6466320352001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17">
+    <row r="16" spans="1:5" ht="17">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
+        <v>2.8876161541123001E-6</v>
+      </c>
+      <c r="D16" s="1">
         <v>8690.4685143093502</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>3220.0367116898901</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17">
+    <row r="17" spans="1:5" ht="17">
       <c r="A17">
         <v>8</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
+        <v>6.4698717013045196E-6</v>
+      </c>
+      <c r="D17" s="1">
         <v>35.823409233631402</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>13.451919553566</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17">
+    <row r="18" spans="1:5" ht="17">
       <c r="A18">
         <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="3">
+        <v>9.1268771912614605E-5</v>
+      </c>
+      <c r="D18" s="1">
         <v>4.8847667814621598</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>2.1979845201460302</v>
       </c>
     </row>

</xml_diff>